<commit_message>
Se agrego el documento de matriz de casos de prueba
</commit_message>
<xml_diff>
--- a/CONTENIDO-PAGINA/Matriz-Code.xlsx
+++ b/CONTENIDO-PAGINA/Matriz-Code.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>IDENTIFICADOR</t>
   </si>
@@ -42,45 +42,6 @@
   </si>
   <si>
     <t>RESULTADO OBTENIDO</t>
-  </si>
-  <si>
-    <t>PRFNL-002</t>
-  </si>
-  <si>
-    <t>PRFNL-003</t>
-  </si>
-  <si>
-    <t>PRFNL-004</t>
-  </si>
-  <si>
-    <t>PRFNL-005</t>
-  </si>
-  <si>
-    <t>PRFNL-006</t>
-  </si>
-  <si>
-    <t>PRFNL-007</t>
-  </si>
-  <si>
-    <t>PRFNL-008</t>
-  </si>
-  <si>
-    <t>PRFNL-009</t>
-  </si>
-  <si>
-    <t>PRFNL-011</t>
-  </si>
-  <si>
-    <t>PRFNL-010</t>
-  </si>
-  <si>
-    <t>Diriga a la pagina principal.</t>
-  </si>
-  <si>
-    <t>1.Ingresar a la pagina inicial.</t>
-  </si>
-  <si>
-    <t>PRNFNL-001</t>
   </si>
   <si>
     <t>Barra de navegación 
@@ -103,22 +64,7 @@
 -Bolsa de trabajo-</t>
   </si>
   <si>
-    <t>Muestre la pantalla de Eventos.</t>
-  </si>
-  <si>
     <t>Muestre la pantalla de Bolsa de trabajo.</t>
-  </si>
-  <si>
-    <t>PRFNL-012</t>
-  </si>
-  <si>
-    <t>PRFNL-013</t>
-  </si>
-  <si>
-    <t>Muestre la ventana de Zologico Zacano.</t>
-  </si>
-  <si>
-    <t>Muestre la ventana de Volcan popocapetetl.</t>
   </si>
   <si>
     <t>Barra de navegación 
@@ -133,9 +79,6 @@
   </si>
   <si>
     <t>Esperado</t>
-  </si>
-  <si>
-    <t>Correcto</t>
   </si>
   <si>
     <t>Ingresar Usuario</t>
@@ -158,12 +101,6 @@
 4.- Dar click izquierdo en "Zologico Zacano"</t>
   </si>
   <si>
-    <t xml:space="preserve">1.- Ingresar a la página incial
-2.- Posicionar el mause sobre el logo del Estado de Mexico
-4.- Dar click izquierdo en el logo del Estado de Mexico.
-</t>
-  </si>
-  <si>
     <t>1.- Ingresar a la página incial
 2.- Posicionar el mause sobre la palabra "Eventos"
 3.- Dar click izquierdo en "Eventos"</t>
@@ -179,33 +116,215 @@
 3.- Dar click izquierdo en "Bolsa de trabajo"</t>
   </si>
   <si>
+    <t>Muestre la pantalla de Historia.</t>
+  </si>
+  <si>
+    <t>Mapa de "Volcan de popocapetetl"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Ingresar a la página incial.
+2.- Dar click  en el logo del Estado de Mexico.
+</t>
+  </si>
+  <si>
+    <t>PEDM-001</t>
+  </si>
+  <si>
+    <t>1.Acceso a la pagina inicial del proyecto.</t>
+  </si>
+  <si>
+    <t>PEDM-002</t>
+  </si>
+  <si>
+    <t>PEDM-003</t>
+  </si>
+  <si>
+    <t>PEDM-004</t>
+  </si>
+  <si>
+    <t>PEDM-005</t>
+  </si>
+  <si>
+    <t>PEDM-006</t>
+  </si>
+  <si>
+    <t>PEDM-007</t>
+  </si>
+  <si>
+    <t>PEDM-008</t>
+  </si>
+  <si>
+    <t>PEDM-009</t>
+  </si>
+  <si>
+    <t>PEDM-010</t>
+  </si>
+  <si>
     <t>1.- Ingresar a la página incial
+2.- Presionar el boton login.
+3.- Ingresar el usuario correcto.
+4.- Ingresar contraseña correcta
+5.- Dar click al botón "Ingresar"</t>
+  </si>
+  <si>
+    <t>1.- Se realizara un login a la pagina.
+2.-Se cambia seccion "login" por el nombre e imagen de perfil del usuario.</t>
+  </si>
+  <si>
+    <t>Diriga a  la ventana de Zologico Zacano.</t>
+  </si>
+  <si>
+    <t>Diriga a la ventana de Volcan popocapetetl.</t>
+  </si>
+  <si>
+    <t>Diriga a  la pantalla de Eventos.</t>
+  </si>
+  <si>
+    <t>1.- Acceso a la pagina inicial del proyecto.
 2.- Tener nombre de usuario y contraseña.</t>
   </si>
   <si>
+    <t>Diriga a la pagina principal del proyecto.</t>
+  </si>
+  <si>
+    <t>Mapa de " Zologico de Zacango".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seccion "Contactanos"
+</t>
+  </si>
+  <si>
+    <t>Seccion "Contactanos"
+-Campo de texto vacio-</t>
+  </si>
+  <si>
+    <t>Seccion "Contactanos"
+-Email sin formato de correo "@, .com"-</t>
+  </si>
+  <si>
+    <t>1.- Acceso a la pagina inicial del proyecto.
+2.- Tener nombre de correo y contraseña.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Ingresar el Nombre,Correo y contraseña y sus dudas o sugerencias.
+4.-Posicionar el mause sobre la palabra "Enviar" 
+5..-Dar click en  la palabra "Enviar"  </t>
+  </si>
+  <si>
+    <t>Mostrara los datos del formulario en la consola del navegador como un objeto de Javascript</t>
+  </si>
+  <si>
+    <t>Mostrara una alerta indicando "Uno de los campos esta vacio"</t>
+  </si>
+  <si>
+    <t>Mostrara una alerta indicando "Ingrese un correo valido"</t>
+  </si>
+  <si>
+    <t>PEDM-013</t>
+  </si>
+  <si>
+    <t>PEDM-012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Dejar alguno de los campos vacios.
+4.-Posicionar el mause sobre la palabra "Enviar" 
+5.-Dar click en  la palabra "Enviar"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Ingresar Nombre,Un email sin formato de correo y su contraseña
+4.-Posicionar el mause sobre la palabra "Enviar" 
+5.-Dar click en  la palabra "Enviar"  </t>
+  </si>
+  <si>
+    <t>PEDM-014</t>
+  </si>
+  <si>
+    <t>PEDM-015</t>
+  </si>
+  <si>
+    <t>PEDM-11</t>
+  </si>
+  <si>
+    <t>"Zologico de Zacango"</t>
+  </si>
+  <si>
+    <t>"Volcan de popocapetetl"</t>
+  </si>
+  <si>
+    <t>"Equinoccio 2021"</t>
+  </si>
+  <si>
+    <t>Diriga a la pagina de "Volcan de popocapetetl"</t>
+  </si>
+  <si>
+    <t>Diriga a la pagina de "Zologico de Zacango"</t>
+  </si>
+  <si>
+    <t>Diriga a la pagina de "Equinoccio 2021"</t>
+  </si>
+  <si>
+    <t>1.Acceso a inicial Equinocciol proyecto.</t>
+  </si>
+  <si>
     <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Login" y clickear
-3.- Clickear el campo de usuario e ingresar elnombre de usuario
-4.- Clickear el campo de contraseña e ingresar la contraseña
-5.- Dar click al botón "Ingresar"</t>
-  </si>
-  <si>
-    <t>Muestre que he iniciado sesión.</t>
-  </si>
-  <si>
-    <t>Muestre la pantalla de Historia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enlaze a el mapa de Zologico de Zacano. </t>
-  </si>
-  <si>
-    <t>Mapa de " Zologico de Zacano".</t>
-  </si>
-  <si>
-    <t>Mapa de "Volcan de popocapetetl"</t>
-  </si>
-  <si>
-    <t>Enlaze a el mapa de Volcan de popocapetetl.</t>
+2.- Deslizar hacia abajo.
+3.- Posicionar el mause sobre la palabra "Zologico de Zacango"
+4.- Dar click.</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Deslizar hacia abajo.
+3.- Posicionar el mause sobre la palabra "Volcan de popocapetetl"
+4.- Dar click.</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Deslizar hacia abajo.
+3.- Posicionar el mause sobre la palabra "Equinoccio 2021"
+4.- Dar click.</t>
+  </si>
+  <si>
+    <t>Enlaze a el mapa de Volcan de popocapetetl y poder explorar en el.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enlaze a el mapa de Zologico de Zacano y poder explorar en el. </t>
+  </si>
+  <si>
+    <t>PEDM-016</t>
+  </si>
+  <si>
+    <t>PEDM-017</t>
+  </si>
+  <si>
+    <t>Mapa de "Equinoccio 2021"</t>
+  </si>
+  <si>
+    <t>Enlaze a el mapa de Equinoccio 2021 y poder navegar en el.</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Posiconar  el mause sobre el mapa de Equinoccio 2021
+4.- Dar click.</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Posiconar  el mause sobre el mapa de Volcan de popocapetetl
+4.- Dar click.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Ingresar a la página incial
+2.- Deslizar hacia el final de la pagina principal.
+3.- Posiconar  el mause sobre el mapa de Zologico de zacango
+4.- Dar click.
+</t>
   </si>
 </sst>
 </file>
@@ -272,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -289,9 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -331,11 +447,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,297 +749,405 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="E3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="E5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>34</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>34</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>34</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="B10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion de matriz de casos de prueba
</commit_message>
<xml_diff>
--- a/CONTENIDO-PAGINA/Matriz-Code.xlsx
+++ b/CONTENIDO-PAGINA/Matriz-Code.xlsx
@@ -84,38 +84,6 @@
     <t>Ingresar Usuario</t>
   </si>
   <si>
-    <t>1.- Posicionar el mouse sobre Lugares Turisticos.
-2.- Dar click izquierdo 
-2.-Posicionar el mouse sobre Volcan popocatepetl.
-2.- Dar click izquierdo .</t>
-  </si>
-  <si>
-    <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Lugares Turisticos"
-3.- Dar click izquierdo en "Lugares Turisticos"</t>
-  </si>
-  <si>
-    <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Lugares Turisticos"
-3.- En linea recta verticalmente, posicionar el mause en el nombre "Zologico Zacano"
-4.- Dar click izquierdo en "Zologico Zacano"</t>
-  </si>
-  <si>
-    <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Eventos"
-3.- Dar click izquierdo en "Eventos"</t>
-  </si>
-  <si>
-    <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Historia"
-3.- Dar click izquierdo en "Historia"</t>
-  </si>
-  <si>
-    <t>1.- Ingresar a la página incial
-2.- Posicionar el mause sobre la palabra "Bolsa de Trabajo"
-3.- Dar click izquierdo en "Bolsa de trabajo"</t>
-  </si>
-  <si>
     <t>Muestre la pantalla de Historia.</t>
   </si>
   <si>
@@ -325,6 +293,38 @@
 3.- Posiconar  el mause sobre el mapa de Zologico de zacango
 4.- Dar click.
 </t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Posicionar el mause sobre la palabra "Lugares Turisticos"
+3.- En linea recta verticalmente, posicionar el mause en el nombre "Zologico Zacano"
+4.- Dar click en "Zologico Zacano"</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Posicionar el mause sobre la palabra "Lugares Turisticos"
+3.- Dar click  en "Lugares Turisticos"</t>
+  </si>
+  <si>
+    <t>1.- Posicionar el mouse sobre Lugares Turisticos.
+2.- Dar click izquierdo 
+2.-Posicionar el mouse sobre Volcan popocatepetl.
+2.- Dar click  .</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Posicionar el mause sobre la palabra "Eventos"
+3.- Dar click en "Eventos"</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Posicionar el mause sobre la palabra "Historia"
+3.- Dar click en "Historia"</t>
+  </si>
+  <si>
+    <t>1.- Ingresar a la página incial
+2.- Posicionar el mause sobre la palabra "Bolsa de Trabajo"
+3.- Dar click en "Bolsa de trabajo"</t>
   </si>
 </sst>
 </file>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,19 +780,19 @@
     </row>
     <row r="2" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>15</v>
@@ -801,16 +801,16 @@
     </row>
     <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>14</v>
@@ -822,19 +822,19 @@
     </row>
     <row r="4" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>15</v>
@@ -843,19 +843,19 @@
     </row>
     <row r="5" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
@@ -864,19 +864,19 @@
     </row>
     <row r="6" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -885,19 +885,19 @@
     </row>
     <row r="7" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>15</v>
@@ -906,16 +906,16 @@
     </row>
     <row r="8" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>11</v>
@@ -927,19 +927,19 @@
     </row>
     <row r="9" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
@@ -948,19 +948,19 @@
     </row>
     <row r="10" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>15</v>
@@ -969,19 +969,19 @@
     </row>
     <row r="11" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
@@ -990,19 +990,19 @@
     </row>
     <row r="12" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
@@ -1011,19 +1011,19 @@
     </row>
     <row r="13" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -1032,19 +1032,19 @@
     </row>
     <row r="14" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
@@ -1053,19 +1053,19 @@
     </row>
     <row r="15" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
@@ -1074,19 +1074,19 @@
     </row>
     <row r="16" spans="1:7" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
@@ -1095,19 +1095,19 @@
     </row>
     <row r="17" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -1116,19 +1116,19 @@
     </row>
     <row r="18" spans="1:7" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>15</v>

</xml_diff>